<commit_message>
for function for adding tenants
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>user@test.com</t>
   </si>
@@ -40,6 +40,39 @@
   </si>
   <si>
     <t>http://www.oxs.co.il</t>
+  </si>
+  <si>
+    <t>add tenants</t>
+  </si>
+  <si>
+    <t>יוסי</t>
+  </si>
+  <si>
+    <t>qa@oxs.co.il</t>
+  </si>
+  <si>
+    <t>משה</t>
+  </si>
+  <si>
+    <t>0524455586</t>
+  </si>
+  <si>
+    <t>דני</t>
+  </si>
+  <si>
+    <t>דוד</t>
+  </si>
+  <si>
+    <t>רמי</t>
+  </si>
+  <si>
+    <t>לאה</t>
+  </si>
+  <si>
+    <t>שרה</t>
+  </si>
+  <si>
+    <t>חוה</t>
   </si>
 </sst>
 </file>
@@ -167,17 +200,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -460,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -471,73 +524,146 @@
     <col min="1" max="1" width="32.25" customWidth="1"/>
     <col min="2" max="2" width="18.125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>123123</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" s="7"/>
+      <c r="D3" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
-        <v>210</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1">
+      <c r="B4" s="7">
+        <v>200</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7">
         <v>5</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7">
         <v>150</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data change & add payment function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -39,9 +39,6 @@
     <t xml:space="preserve">login </t>
   </si>
   <si>
-    <t>http://www.oxs.co.il</t>
-  </si>
-  <si>
     <t>add tenants</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>חוה</t>
+  </si>
+  <si>
+    <t>https://stg.oxs.co.il/</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -538,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -552,7 +552,7 @@
         <v>200</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -564,19 +564,19 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7">
         <v>200</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -586,7 +586,7 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -596,7 +596,7 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -604,7 +604,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -612,7 +612,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -620,7 +620,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -628,7 +628,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -636,7 +636,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>